<commit_message>
analysis results added and fuux bugs on execution time computing
</commit_message>
<xml_diff>
--- a/output/ParallelSortingResults.xlsx
+++ b/output/ParallelSortingResults.xlsx
@@ -92,7 +92,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0">
-        <v>0.002539</v>
+        <v>0.0808664</v>
       </c>
     </row>
     <row r="3">
@@ -100,7 +100,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0">
-        <v>0.0013846</v>
+        <v>0.0933394</v>
       </c>
     </row>
     <row r="4">
@@ -108,7 +108,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="0">
-        <v>0.0064659</v>
+        <v>0.0991365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated new data set and analyze the output results
</commit_message>
<xml_diff>
--- a/output/ParallelSortingResults.xlsx
+++ b/output/ParallelSortingResults.xlsx
@@ -92,7 +92,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0">
-        <v>0.0808664</v>
+        <v>0.9571592</v>
       </c>
     </row>
     <row r="3">
@@ -100,7 +100,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0">
-        <v>0.0933394</v>
+        <v>2.9498729</v>
       </c>
     </row>
     <row r="4">
@@ -108,7 +108,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="0">
-        <v>0.0991365</v>
+        <v>0.2342423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>